<commit_message>
Polish names -> English names
</commit_message>
<xml_diff>
--- a/Data/Kolchicyna_prepared_data.xlsx
+++ b/Data/Kolchicyna_prepared_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\GitHub\Kolchicyna\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\GitHub\GitHub - Colchicine ML\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2992BB-D95E-4D84-9108-847C6D56FCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FEDD1D-882A-41BC-93E9-AC306DFAC6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,18 +35,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="284">
   <si>
-    <t>Publikacja DOI</t>
-  </si>
-  <si>
-    <t>Numer związku w publikacji</t>
-  </si>
-  <si>
     <t>SMILES</t>
   </si>
   <si>
-    <t>Atywność [nM]</t>
-  </si>
-  <si>
     <t>A549</t>
   </si>
   <si>
@@ -885,6 +876,15 @@
   </si>
   <si>
     <t xml:space="preserve">67,0 </t>
+  </si>
+  <si>
+    <t>Publication DOI</t>
+  </si>
+  <si>
+    <t>Number of compound in publication</t>
+  </si>
+  <si>
+    <t>Activity [nM]</t>
   </si>
 </sst>
 </file>
@@ -979,9 +979,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1019,9 +1019,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1054,26 +1054,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1106,26 +1089,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1302,7 +1268,7 @@
   <dimension ref="A1:O121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="E2" sqref="E2:E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,46 +1281,46 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1362,31 +1328,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K2">
         <v>10.8</v>
@@ -1409,25 +1375,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I3">
         <v>31.1</v>
@@ -1456,31 +1422,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K4">
         <v>10.9</v>
@@ -1503,31 +1469,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K5">
         <v>10.5</v>
@@ -1550,31 +1516,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K6">
         <v>89.5</v>
@@ -1597,31 +1563,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K7">
         <v>13.1</v>
@@ -1644,28 +1610,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J8">
         <v>106.7</v>
@@ -1691,28 +1657,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="J9">
         <v>78.5</v>
@@ -1738,28 +1704,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G10">
         <v>1124.4000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J10">
         <v>1036.3</v>
@@ -1785,31 +1751,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I11">
         <v>1984.1</v>
       </c>
       <c r="J11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="K11">
         <v>151.80000000000001</v>
@@ -1832,31 +1798,31 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="J12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="K12">
         <v>9.6</v>
@@ -1879,31 +1845,31 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G13">
         <v>9.6999999999999993</v>
       </c>
       <c r="H13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="J13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K13">
         <v>10.9</v>
@@ -1926,31 +1892,31 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K14">
         <v>9.3000000000000007</v>
@@ -1973,31 +1939,31 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K15">
         <v>10.8</v>
@@ -2020,25 +1986,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I16">
         <v>85.6</v>
@@ -2067,31 +2033,31 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I17" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J17" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="K17">
         <v>83.4</v>
@@ -2114,31 +2080,31 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F18">
         <v>9.6</v>
       </c>
       <c r="G18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K18">
         <v>9.6</v>
@@ -2161,31 +2127,31 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K19">
         <v>70.5</v>
@@ -2208,31 +2174,31 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H20" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="J20" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K20">
         <v>101.2</v>
@@ -2255,31 +2221,31 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K21">
         <v>10.7</v>
@@ -2302,31 +2268,31 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I22">
         <v>210.5</v>
       </c>
       <c r="J22" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="K22">
         <v>95</v>
@@ -2349,31 +2315,31 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H23" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K23">
         <v>47.3</v>
@@ -2396,31 +2362,31 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G24" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H24" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I24" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J24" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="K24">
         <v>19.3</v>
@@ -2443,31 +2409,31 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G25" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I25" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K25">
         <v>0.9</v>
@@ -2490,31 +2456,31 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I26" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J26" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="K26">
         <v>11</v>
@@ -2537,16 +2503,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F27">
         <v>12986</v>
@@ -2578,16 +2544,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F28">
         <v>12469</v>
@@ -2619,16 +2585,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F29">
         <v>9970</v>
@@ -2660,16 +2626,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F30">
         <v>20387</v>
@@ -2701,16 +2667,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F31">
         <v>8750</v>
@@ -2742,16 +2708,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F32">
         <v>978</v>
@@ -2783,16 +2749,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F33">
         <v>9671</v>
@@ -2824,16 +2790,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F34">
         <v>823</v>
@@ -2865,16 +2831,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F35">
         <v>482</v>
@@ -2906,16 +2872,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F36">
         <v>971</v>
@@ -2947,16 +2913,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F37">
         <v>885</v>
@@ -2988,16 +2954,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F38">
         <v>601</v>
@@ -3029,16 +2995,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F39">
         <v>900</v>
@@ -3070,16 +3036,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F40">
         <v>955</v>
@@ -3111,16 +3077,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F41">
         <v>4.4000000000000004</v>
@@ -3158,16 +3124,16 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F42">
         <v>12</v>
@@ -3205,16 +3171,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F43">
         <v>1.4</v>
@@ -3252,16 +3218,16 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C44">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E44" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F44">
         <v>6.1</v>
@@ -3299,16 +3265,16 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C45">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E45" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F45">
         <v>15</v>
@@ -3346,16 +3312,16 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C46">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F46">
         <v>6.4</v>
@@ -3393,16 +3359,16 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C47">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F47">
         <v>70</v>
@@ -3440,16 +3406,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F48">
         <v>12</v>
@@ -3487,16 +3453,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C49">
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E49" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F49">
         <v>13</v>
@@ -3534,16 +3500,16 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C50">
         <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F50">
         <v>14</v>
@@ -3581,16 +3547,16 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C51">
         <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F51">
         <v>37</v>
@@ -3628,16 +3594,16 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C52">
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E52" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F52">
         <v>94</v>
@@ -3675,16 +3641,16 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C53">
         <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E53" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F53">
         <v>13</v>
@@ -3722,16 +3688,16 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C54">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E54" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F54">
         <v>39</v>
@@ -3769,16 +3735,16 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C55">
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F55">
         <v>35</v>
@@ -3816,16 +3782,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C56">
         <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E56" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F56">
         <v>6.9</v>
@@ -3863,16 +3829,16 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C57">
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E57" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F57">
         <v>13</v>
@@ -3910,16 +3876,16 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C58">
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E58" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F58">
         <v>17</v>
@@ -3957,16 +3923,16 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C59">
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E59" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F59">
         <v>1300</v>
@@ -4004,16 +3970,16 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C60">
         <v>21</v>
       </c>
       <c r="D60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F60">
         <v>21</v>
@@ -4051,16 +4017,16 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C61">
         <v>22</v>
       </c>
       <c r="D61" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F61">
         <v>72</v>
@@ -4098,16 +4064,16 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C62">
         <v>23</v>
       </c>
       <c r="D62" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E62" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F62">
         <v>1000</v>
@@ -4145,16 +4111,16 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C63">
         <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E63" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F63">
         <v>16</v>
@@ -4192,16 +4158,16 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C64">
         <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E64" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F64">
         <v>1.3</v>
@@ -4239,16 +4205,16 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C65">
         <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F65">
         <v>2.4</v>
@@ -4286,16 +4252,16 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C66">
         <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E66" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F66">
         <v>2.9</v>
@@ -4333,16 +4299,16 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C67">
         <v>28</v>
       </c>
       <c r="D67" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E67" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F67">
         <v>9.5</v>
@@ -4380,16 +4346,16 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C68">
         <v>29</v>
       </c>
       <c r="D68" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E68" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F68">
         <v>12</v>
@@ -4427,16 +4393,16 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C69">
         <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E69" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F69">
         <v>16</v>
@@ -4474,16 +4440,16 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C70">
         <v>31</v>
       </c>
       <c r="D70" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E70" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F70">
         <v>3.3</v>
@@ -4521,16 +4487,16 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C71">
         <v>32</v>
       </c>
       <c r="D71" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E71" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F71">
         <v>4.4000000000000004</v>
@@ -4568,16 +4534,16 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C72">
         <v>33</v>
       </c>
       <c r="D72" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E72" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F72">
         <v>11</v>
@@ -4615,16 +4581,16 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C73">
         <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E73" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F73">
         <v>26</v>
@@ -4662,16 +4628,16 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C74">
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E74" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F74">
         <v>5.7</v>
@@ -4709,16 +4675,16 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C75">
         <v>36</v>
       </c>
       <c r="D75" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E75" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F75">
         <v>22</v>
@@ -4756,16 +4722,16 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C76">
         <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E76" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F76">
         <v>7.2</v>
@@ -4803,16 +4769,16 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C77">
         <v>38</v>
       </c>
       <c r="D77" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E77" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F77">
         <v>4.8</v>
@@ -4850,16 +4816,16 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E78" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F78">
         <v>3.3</v>
@@ -4897,16 +4863,16 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C79">
         <v>40</v>
       </c>
       <c r="D79" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E79" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F79">
         <v>1.2</v>
@@ -4944,16 +4910,16 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>41</v>
       </c>
       <c r="D80" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E80" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F80">
         <v>5.4</v>
@@ -4991,16 +4957,16 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C81">
         <v>42</v>
       </c>
       <c r="D81" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E81" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F81">
         <v>1.9</v>
@@ -5038,16 +5004,16 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>43</v>
       </c>
       <c r="D82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F82">
         <v>4.0999999999999996</v>
@@ -5085,16 +5051,16 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C83">
         <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E83" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F83">
         <v>9.4</v>
@@ -5132,16 +5098,16 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C84">
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E84" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F84">
         <v>10.5</v>
@@ -5179,16 +5145,16 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C85">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E85" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F85">
         <v>8.1</v>
@@ -5226,16 +5192,16 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C86">
         <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E86" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F86">
         <v>88.4</v>
@@ -5273,16 +5239,16 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C87">
         <v>8</v>
       </c>
       <c r="D87" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E87" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F87">
         <v>9.6</v>
@@ -5320,16 +5286,16 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C88">
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E88" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F88">
         <v>9.1999999999999993</v>
@@ -5367,16 +5333,16 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C89">
         <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E89" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F89">
         <v>9</v>
@@ -5414,16 +5380,16 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C90">
         <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E90" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F90">
         <v>8.4</v>
@@ -5461,16 +5427,16 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C91">
         <v>12</v>
       </c>
       <c r="D91" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E91" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F91">
         <v>9.5</v>
@@ -5508,16 +5474,16 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C92">
         <v>13</v>
       </c>
       <c r="D92" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E92" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F92">
         <v>4.5999999999999996</v>
@@ -5555,16 +5521,16 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C93">
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E93" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F93">
         <v>1.1000000000000001</v>
@@ -5602,16 +5568,16 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C94">
         <v>15</v>
       </c>
       <c r="D94" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E94" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F94">
         <v>8.9</v>
@@ -5649,16 +5615,16 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C95">
         <v>16</v>
       </c>
       <c r="D95" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E95" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F95">
         <v>8.9</v>
@@ -5696,16 +5662,16 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C96">
         <v>17</v>
       </c>
       <c r="D96" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E96" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F96">
         <v>9.4</v>
@@ -5743,25 +5709,25 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C97">
         <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E97" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F97" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G97" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H97" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I97">
         <v>6300</v>
@@ -5790,31 +5756,31 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C98">
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E98" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F98" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G98" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H98" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I98">
         <v>7300</v>
       </c>
       <c r="J98" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K98">
         <v>79</v>
@@ -5837,22 +5803,22 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C99">
         <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E99" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F99" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G99" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H99">
         <v>24</v>
@@ -5861,7 +5827,7 @@
         <v>2400</v>
       </c>
       <c r="J99" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K99">
         <v>34</v>
@@ -5884,31 +5850,31 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C100">
         <v>7</v>
       </c>
       <c r="D100" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E100" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F100" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G100" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H100" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I100">
         <v>1600</v>
       </c>
       <c r="J100" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K100">
         <v>33</v>
@@ -5931,31 +5897,31 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C101">
         <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E101" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F101">
         <v>110</v>
       </c>
       <c r="G101" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H101" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I101">
         <v>1200</v>
       </c>
       <c r="J101" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K101">
         <v>110</v>
@@ -5978,25 +5944,25 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C102">
         <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E102" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F102" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G102" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H102" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I102">
         <v>730</v>
@@ -6025,16 +5991,16 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C103">
         <v>10</v>
       </c>
       <c r="D103" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E103" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F103">
         <v>190</v>
@@ -6043,7 +6009,7 @@
         <v>120</v>
       </c>
       <c r="H103" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I103">
         <v>10000</v>
@@ -6072,31 +6038,31 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C104">
         <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E104" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F104" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G104" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H104" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I104">
         <v>1100</v>
       </c>
       <c r="J104" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K104">
         <v>12</v>
@@ -6119,25 +6085,25 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C105">
         <v>12</v>
       </c>
       <c r="D105" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E105" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F105" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G105" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H105" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I105">
         <v>1000</v>
@@ -6166,25 +6132,25 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C106">
         <v>13</v>
       </c>
       <c r="D106" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E106" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F106" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G106" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H106" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I106">
         <v>1000</v>
@@ -6213,31 +6179,31 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C107">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E107" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F107" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G107">
         <v>130</v>
       </c>
       <c r="H107" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I107">
         <v>1000</v>
       </c>
       <c r="J107" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K107">
         <v>82</v>
@@ -6260,25 +6226,25 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C108">
         <v>15</v>
       </c>
       <c r="D108" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E108" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F108" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G108" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H108" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I108">
         <v>1400</v>
@@ -6307,31 +6273,31 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C109">
         <v>16</v>
       </c>
       <c r="D109" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E109" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F109" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G109" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H109" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I109">
         <v>1000</v>
       </c>
       <c r="J109" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K109">
         <v>2</v>
@@ -6354,22 +6320,22 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C110">
         <v>17</v>
       </c>
       <c r="D110" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E110" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F110">
         <v>13</v>
       </c>
       <c r="G110" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H110">
         <v>9.4</v>
@@ -6378,7 +6344,7 @@
         <v>700</v>
       </c>
       <c r="J110" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K110">
         <v>13</v>
@@ -6401,22 +6367,22 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C111">
         <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E111" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F111">
         <v>13</v>
       </c>
       <c r="G111" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H111">
         <v>13</v>
@@ -6425,7 +6391,7 @@
         <v>200</v>
       </c>
       <c r="J111" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="K111">
         <v>13</v>
@@ -6448,22 +6414,22 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C112">
         <v>19</v>
       </c>
       <c r="D112" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E112" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F112" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G112" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H112">
         <v>16</v>
@@ -6472,7 +6438,7 @@
         <v>860</v>
       </c>
       <c r="J112" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K112">
         <v>78</v>
@@ -6495,31 +6461,31 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C113">
         <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E113" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F113" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G113" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H113" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I113">
         <v>140</v>
       </c>
       <c r="J113" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K113">
         <v>23</v>
@@ -6542,31 +6508,31 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C114">
         <v>21</v>
       </c>
       <c r="D114" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E114" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F114" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G114" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H114" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I114">
         <v>140</v>
       </c>
       <c r="J114" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K114">
         <v>27</v>
@@ -6589,31 +6555,31 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C115">
         <v>22</v>
       </c>
       <c r="D115" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E115" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F115" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G115" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H115" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I115">
         <v>160</v>
       </c>
       <c r="J115" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K115">
         <v>15</v>
@@ -6636,25 +6602,25 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C116">
         <v>23</v>
       </c>
       <c r="D116" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E116" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F116" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G116" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H116" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I116">
         <v>940</v>
@@ -6683,31 +6649,31 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C117">
         <v>24</v>
       </c>
       <c r="D117" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E117" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F117" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G117">
         <v>120</v>
       </c>
       <c r="H117" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I117">
         <v>2700</v>
       </c>
       <c r="J117" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="K117">
         <v>86</v>
@@ -6730,25 +6696,25 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C118">
         <v>25</v>
       </c>
       <c r="D118" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E118" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F118" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G118" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H118" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I118">
         <v>5300</v>
@@ -6777,16 +6743,16 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C119">
         <v>26</v>
       </c>
       <c r="D119" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E119" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F119">
         <v>930</v>
@@ -6824,16 +6790,16 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C120">
         <v>27</v>
       </c>
       <c r="D120" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E120" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F120">
         <v>850</v>
@@ -6871,16 +6837,16 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C121">
         <v>28</v>
       </c>
       <c r="D121" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E121" t="s">
-        <v>3</v>
+        <v>283</v>
       </c>
       <c r="F121">
         <v>740</v>
@@ -7024,5 +6990,6 @@
     <hyperlink ref="B121" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId108"/>
 </worksheet>
 </file>
</xml_diff>